<commit_message>
updated master amb mapping files
</commit_message>
<xml_diff>
--- a/master_amb_mapping_updated.xlsx
+++ b/master_amb_mapping_updated.xlsx
@@ -13,9 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$1864</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$1865</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10726" uniqueCount="2209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10774" uniqueCount="2210">
   <si>
     <t>CAMPUS</t>
   </si>
@@ -6654,6 +6655,9 @@
   </si>
   <si>
     <t>MS NOW</t>
+  </si>
+  <si>
+    <t>4982 HYLAN BLVD THORACIC SURGERY</t>
   </si>
 </sst>
 </file>
@@ -7004,8 +7008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1865"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7013,7 +7017,7 @@
     <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.85546875" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="36.7109375" customWidth="1"/>
@@ -8035,15 +8039,17 @@
         <v>37</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="E34" s="1">
-        <v>4100999</v>
-      </c>
-      <c r="F34" s="1"/>
+        <v>8823014</v>
+      </c>
+      <c r="F34" s="4">
+        <v>45093.489583333336</v>
+      </c>
       <c r="G34" s="1" t="s">
         <v>39</v>
       </c>
@@ -8866,16 +8872,16 @@
         <v>37</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E59" s="1">
-        <v>8823014</v>
+        <v>8823015</v>
       </c>
       <c r="F59" s="4">
-        <v>45093.489583333336</v>
+        <v>45093.583333333336</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>39</v>
@@ -8899,16 +8905,16 @@
         <v>37</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>107</v>
+        <v>224</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>106</v>
+        <v>224</v>
       </c>
       <c r="E60" s="1">
-        <v>41001041</v>
+        <v>8823041</v>
       </c>
       <c r="F60" s="4">
-        <v>44386.6875</v>
+        <v>45093.645833333336</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>39</v>
@@ -8926,22 +8932,22 @@
     </row>
     <row r="61" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>2202</v>
+        <v>2200</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>37</v>
+        <v>521</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>108</v>
+        <v>522</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>108</v>
+        <v>522</v>
       </c>
       <c r="E61" s="1">
-        <v>8823015</v>
+        <v>8011005</v>
       </c>
       <c r="F61" s="4">
-        <v>45093.583333333336</v>
+        <v>45093.680555555555</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>39</v>
@@ -11396,22 +11402,22 @@
     </row>
     <row r="137" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>2202</v>
+        <v>2200</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>37</v>
+        <v>523</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>224</v>
+        <v>524</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>224</v>
+        <v>524</v>
       </c>
       <c r="E137" s="1">
-        <v>8823041</v>
+        <v>8011006</v>
       </c>
       <c r="F137" s="4">
-        <v>45093.645833333336</v>
+        <v>45093.625</v>
       </c>
       <c r="G137" s="1" t="s">
         <v>39</v>
@@ -11429,22 +11435,22 @@
     </row>
     <row r="138" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>2202</v>
+        <v>2200</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>225</v>
+        <v>680</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>224</v>
+        <v>680</v>
       </c>
       <c r="E138" s="1">
-        <v>41001046</v>
+        <v>8004026</v>
       </c>
       <c r="F138" s="4">
-        <v>44386.645833333336</v>
+        <v>45093.375</v>
       </c>
       <c r="G138" s="1" t="s">
         <v>39</v>
@@ -13595,22 +13601,22 @@
     </row>
     <row r="206" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>276</v>
+        <v>2200</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>310</v>
+        <v>695</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>311</v>
+        <v>695</v>
       </c>
       <c r="E206" s="1">
-        <v>8802058</v>
+        <v>8005002</v>
       </c>
       <c r="F206" s="4">
-        <v>44894.649305555555</v>
+        <v>45096.645833333336</v>
       </c>
       <c r="G206" s="1" t="s">
         <v>39</v>
@@ -13628,22 +13634,22 @@
     </row>
     <row r="207" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>276</v>
+        <v>12</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>310</v>
+        <v>1147</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>311</v>
+        <v>1147</v>
       </c>
       <c r="E207" s="1">
-        <v>43001051</v>
+        <v>8811002</v>
       </c>
       <c r="F207" s="4">
-        <v>44386.354166666664</v>
+        <v>45093.625</v>
       </c>
       <c r="G207" s="1" t="s">
         <v>39</v>
@@ -19007,22 +19013,22 @@
     </row>
     <row r="386" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>2200</v>
+        <v>51</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>521</v>
+        <v>37</v>
       </c>
       <c r="C386" s="1" t="s">
-        <v>522</v>
+        <v>1207</v>
       </c>
       <c r="D386" s="1" t="s">
-        <v>522</v>
+        <v>1207</v>
       </c>
       <c r="E386" s="1">
-        <v>8011005</v>
+        <v>8881007</v>
       </c>
       <c r="F386" s="4">
-        <v>45093.680555555555</v>
+        <v>45093.6875</v>
       </c>
       <c r="G386" s="1" t="s">
         <v>39</v>
@@ -19040,22 +19046,22 @@
     </row>
     <row r="387" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
-        <v>2200</v>
+        <v>51</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>523</v>
+        <v>37</v>
       </c>
       <c r="C387" s="1" t="s">
-        <v>524</v>
+        <v>1209</v>
       </c>
       <c r="D387" s="1" t="s">
-        <v>524</v>
+        <v>1209</v>
       </c>
       <c r="E387" s="1">
-        <v>8011006</v>
+        <v>8881008</v>
       </c>
       <c r="F387" s="4">
-        <v>45093.625</v>
+        <v>45093.666666666664</v>
       </c>
       <c r="G387" s="1" t="s">
         <v>39</v>
@@ -19065,7 +19071,7 @@
         <v>23</v>
       </c>
       <c r="J387" s="1" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="K387" s="1"/>
       <c r="L387" s="1"/>
@@ -23145,22 +23151,22 @@
     </row>
     <row r="522" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A522" s="1" t="s">
-        <v>2200</v>
+        <v>51</v>
       </c>
       <c r="B522" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C522" s="1" t="s">
-        <v>680</v>
+        <v>1213</v>
       </c>
       <c r="D522" s="1" t="s">
-        <v>680</v>
+        <v>1213</v>
       </c>
       <c r="E522" s="1">
-        <v>8004026</v>
+        <v>8881010</v>
       </c>
       <c r="F522" s="4">
-        <v>45093.375</v>
+        <v>45093.625</v>
       </c>
       <c r="G522" s="1" t="s">
         <v>39</v>
@@ -23170,7 +23176,7 @@
         <v>23</v>
       </c>
       <c r="J522" s="1" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="K522" s="1"/>
       <c r="L522" s="1"/>
@@ -23578,22 +23584,22 @@
     </row>
     <row r="535" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A535" s="1" t="s">
-        <v>2200</v>
+        <v>51</v>
       </c>
       <c r="B535" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C535" s="1" t="s">
-        <v>695</v>
+        <v>1226</v>
       </c>
       <c r="D535" s="1" t="s">
-        <v>695</v>
+        <v>1226</v>
       </c>
       <c r="E535" s="1">
-        <v>8005002</v>
+        <v>8881009</v>
       </c>
       <c r="F535" s="4">
-        <v>45096.645833333336</v>
+        <v>45000.354166666664</v>
       </c>
       <c r="G535" s="1" t="s">
         <v>39</v>
@@ -23603,7 +23609,7 @@
         <v>23</v>
       </c>
       <c r="J535" s="1" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="K535" s="1"/>
       <c r="L535" s="1"/>
@@ -35596,22 +35602,22 @@
     </row>
     <row r="939" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A939" s="1" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B939" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C939" s="1" t="s">
-        <v>1147</v>
+        <v>1228</v>
       </c>
       <c r="D939" s="1" t="s">
-        <v>1147</v>
+        <v>1228</v>
       </c>
       <c r="E939" s="1">
-        <v>8811002</v>
+        <v>8881011</v>
       </c>
       <c r="F939" s="4">
-        <v>45093.625</v>
+        <v>44862.541666666664</v>
       </c>
       <c r="G939" s="1" t="s">
         <v>39</v>
@@ -35621,7 +35627,7 @@
         <v>23</v>
       </c>
       <c r="J939" s="1" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="K939" s="1"/>
       <c r="L939" s="1"/>
@@ -36797,25 +36803,29 @@
     </row>
     <row r="980" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A980" s="1" t="s">
-        <v>51</v>
+        <v>276</v>
       </c>
       <c r="B980" s="1" t="s">
-        <v>37</v>
+        <v>406</v>
       </c>
       <c r="C980" s="1" t="s">
-        <v>1197</v>
+        <v>1365</v>
       </c>
       <c r="D980" s="1" t="s">
-        <v>1198</v>
+        <v>1365</v>
       </c>
       <c r="E980" s="1">
-        <v>4100901</v>
-      </c>
-      <c r="F980" s="1"/>
+        <v>8899006</v>
+      </c>
+      <c r="F980" s="4">
+        <v>45092.666666666664</v>
+      </c>
       <c r="G980" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H980" s="1"/>
+      <c r="H980" s="1" t="s">
+        <v>2199</v>
+      </c>
       <c r="I980" s="1" t="s">
         <v>23</v>
       </c>
@@ -37059,22 +37069,22 @@
     </row>
     <row r="988" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A988" s="1" t="s">
-        <v>51</v>
+        <v>276</v>
       </c>
       <c r="B988" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C988" s="1" t="s">
-        <v>1207</v>
+        <v>1366</v>
       </c>
       <c r="D988" s="1" t="s">
-        <v>1207</v>
+        <v>1366</v>
       </c>
       <c r="E988" s="1">
-        <v>8881007</v>
+        <v>8805016</v>
       </c>
       <c r="F988" s="4">
-        <v>45093.6875</v>
+        <v>45093.635416666664</v>
       </c>
       <c r="G988" s="1" t="s">
         <v>39</v>
@@ -37092,22 +37102,22 @@
     </row>
     <row r="989" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A989" s="1" t="s">
-        <v>51</v>
+        <v>276</v>
       </c>
       <c r="B989" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C989" s="1" t="s">
-        <v>1208</v>
+        <v>1386</v>
       </c>
       <c r="D989" s="1" t="s">
-        <v>1207</v>
+        <v>1386</v>
       </c>
       <c r="E989" s="1">
-        <v>41082007</v>
+        <v>8899003</v>
       </c>
       <c r="F989" s="4">
-        <v>44386.677083333336</v>
+        <v>45093.625</v>
       </c>
       <c r="G989" s="1" t="s">
         <v>39</v>
@@ -37117,7 +37127,7 @@
         <v>23</v>
       </c>
       <c r="J989" s="1" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="K989" s="1"/>
       <c r="L989" s="1"/>
@@ -37125,22 +37135,22 @@
     </row>
     <row r="990" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A990" s="1" t="s">
-        <v>51</v>
+        <v>276</v>
       </c>
       <c r="B990" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C990" s="1" t="s">
-        <v>1209</v>
+        <v>1391</v>
       </c>
       <c r="D990" s="1" t="s">
-        <v>1209</v>
+        <v>1391</v>
       </c>
       <c r="E990" s="1">
-        <v>8881008</v>
+        <v>8899004</v>
       </c>
       <c r="F990" s="4">
-        <v>45093.666666666664</v>
+        <v>45093.5625</v>
       </c>
       <c r="G990" s="1" t="s">
         <v>39</v>
@@ -37158,22 +37168,22 @@
     </row>
     <row r="991" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A991" s="1" t="s">
-        <v>51</v>
+        <v>2203</v>
       </c>
       <c r="B991" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C991" s="1" t="s">
-        <v>1210</v>
+        <v>1423</v>
       </c>
       <c r="D991" s="1" t="s">
-        <v>1209</v>
+        <v>1423</v>
       </c>
       <c r="E991" s="1">
-        <v>41082008</v>
+        <v>8808037</v>
       </c>
       <c r="F991" s="4">
-        <v>44386.645833333336</v>
+        <v>45093.666666666664</v>
       </c>
       <c r="G991" s="1" t="s">
         <v>39</v>
@@ -37261,19 +37271,19 @@
     </row>
     <row r="994" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A994" s="1" t="s">
-        <v>51</v>
+        <v>2203</v>
       </c>
       <c r="B994" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C994" s="1" t="s">
-        <v>1213</v>
+        <v>1429</v>
       </c>
       <c r="D994" s="1" t="s">
-        <v>1213</v>
+        <v>1429</v>
       </c>
       <c r="E994" s="1">
-        <v>8881010</v>
+        <v>8808013</v>
       </c>
       <c r="F994" s="4">
         <v>45093.625</v>
@@ -37294,22 +37304,22 @@
     </row>
     <row r="995" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A995" s="1" t="s">
-        <v>51</v>
+        <v>2203</v>
       </c>
       <c r="B995" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C995" s="1" t="s">
-        <v>1214</v>
+        <v>1484</v>
       </c>
       <c r="D995" s="1" t="s">
-        <v>1213</v>
+        <v>1484</v>
       </c>
       <c r="E995" s="1">
-        <v>41082010</v>
+        <v>8808038</v>
       </c>
       <c r="F995" s="4">
-        <v>44386.677083333336</v>
+        <v>45093.416666666664</v>
       </c>
       <c r="G995" s="1" t="s">
         <v>39</v>
@@ -37680,23 +37690,21 @@
     </row>
     <row r="1007" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1007" s="1" t="s">
-        <v>51</v>
+        <v>2202</v>
       </c>
       <c r="B1007" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1007" s="1" t="s">
-        <v>1226</v>
+        <v>75</v>
       </c>
       <c r="D1007" s="1" t="s">
-        <v>1226</v>
+        <v>76</v>
       </c>
       <c r="E1007" s="1">
-        <v>8881009</v>
-      </c>
-      <c r="F1007" s="4">
-        <v>45000.354166666664</v>
-      </c>
+        <v>4100999</v>
+      </c>
+      <c r="F1007" s="1"/>
       <c r="G1007" s="1" t="s">
         <v>39</v>
       </c>
@@ -37705,7 +37713,7 @@
         <v>23</v>
       </c>
       <c r="J1007" s="1" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="K1007" s="1"/>
       <c r="L1007" s="1"/>
@@ -37713,22 +37721,22 @@
     </row>
     <row r="1008" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1008" s="1" t="s">
-        <v>51</v>
+        <v>2202</v>
       </c>
       <c r="B1008" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1008" s="1" t="s">
-        <v>1227</v>
+        <v>107</v>
       </c>
       <c r="D1008" s="1" t="s">
-        <v>1226</v>
+        <v>106</v>
       </c>
       <c r="E1008" s="1">
-        <v>41082009</v>
+        <v>41001041</v>
       </c>
       <c r="F1008" s="4">
-        <v>44386.604166666664</v>
+        <v>44386.6875</v>
       </c>
       <c r="G1008" s="1" t="s">
         <v>39</v>
@@ -37746,22 +37754,22 @@
     </row>
     <row r="1009" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1009" s="1" t="s">
-        <v>51</v>
+        <v>2202</v>
       </c>
       <c r="B1009" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1009" s="1" t="s">
-        <v>1228</v>
+        <v>225</v>
       </c>
       <c r="D1009" s="1" t="s">
-        <v>1228</v>
+        <v>224</v>
       </c>
       <c r="E1009" s="1">
-        <v>8881011</v>
+        <v>41001046</v>
       </c>
       <c r="F1009" s="4">
-        <v>44862.541666666664</v>
+        <v>44386.645833333336</v>
       </c>
       <c r="G1009" s="1" t="s">
         <v>39</v>
@@ -37771,7 +37779,7 @@
         <v>23</v>
       </c>
       <c r="J1009" s="1" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="K1009" s="1"/>
       <c r="L1009" s="1"/>
@@ -37779,22 +37787,22 @@
     </row>
     <row r="1010" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1010" s="1" t="s">
-        <v>51</v>
+        <v>276</v>
       </c>
       <c r="B1010" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1010" s="1" t="s">
-        <v>1229</v>
+        <v>310</v>
       </c>
       <c r="D1010" s="1" t="s">
-        <v>1228</v>
+        <v>311</v>
       </c>
       <c r="E1010" s="1">
-        <v>41082011</v>
+        <v>8802058</v>
       </c>
       <c r="F1010" s="4">
-        <v>44385.385416666664</v>
+        <v>44894.649305555555</v>
       </c>
       <c r="G1010" s="1" t="s">
         <v>39</v>
@@ -41717,26 +41725,24 @@
         <v>276</v>
       </c>
       <c r="B1139" s="1" t="s">
-        <v>406</v>
+        <v>37</v>
       </c>
       <c r="C1139" s="1" t="s">
-        <v>1365</v>
+        <v>310</v>
       </c>
       <c r="D1139" s="1" t="s">
-        <v>1365</v>
+        <v>311</v>
       </c>
       <c r="E1139" s="1">
-        <v>8899006</v>
+        <v>43001051</v>
       </c>
       <c r="F1139" s="4">
-        <v>45092.666666666664</v>
+        <v>44386.354166666664</v>
       </c>
       <c r="G1139" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H1139" s="1" t="s">
-        <v>2199</v>
-      </c>
+      <c r="H1139" s="1"/>
       <c r="I1139" s="1" t="s">
         <v>23</v>
       </c>
@@ -41749,23 +41755,21 @@
     </row>
     <row r="1140" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1140" s="1" t="s">
-        <v>276</v>
+        <v>51</v>
       </c>
       <c r="B1140" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1140" s="1" t="s">
-        <v>1366</v>
+        <v>1197</v>
       </c>
       <c r="D1140" s="1" t="s">
-        <v>1366</v>
+        <v>1198</v>
       </c>
       <c r="E1140" s="1">
-        <v>8805016</v>
-      </c>
-      <c r="F1140" s="4">
-        <v>45093.635416666664</v>
-      </c>
+        <v>4100901</v>
+      </c>
+      <c r="F1140" s="1"/>
       <c r="G1140" s="1" t="s">
         <v>39</v>
       </c>
@@ -42347,22 +42351,22 @@
     </row>
     <row r="1158" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1158" s="1" t="s">
-        <v>276</v>
+        <v>51</v>
       </c>
       <c r="B1158" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1158" s="1" t="s">
-        <v>1386</v>
+        <v>1210</v>
       </c>
       <c r="D1158" s="1" t="s">
-        <v>1386</v>
+        <v>1209</v>
       </c>
       <c r="E1158" s="1">
-        <v>8899003</v>
+        <v>41082008</v>
       </c>
       <c r="F1158" s="4">
-        <v>45093.625</v>
+        <v>44386.645833333336</v>
       </c>
       <c r="G1158" s="1" t="s">
         <v>39</v>
@@ -42372,7 +42376,7 @@
         <v>23</v>
       </c>
       <c r="J1158" s="1" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="K1158" s="1"/>
       <c r="L1158" s="1"/>
@@ -42380,22 +42384,22 @@
     </row>
     <row r="1159" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1159" s="1" t="s">
-        <v>276</v>
+        <v>51</v>
       </c>
       <c r="B1159" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1159" s="1" t="s">
-        <v>1387</v>
+        <v>1208</v>
       </c>
       <c r="D1159" s="1" t="s">
-        <v>1386</v>
+        <v>1207</v>
       </c>
       <c r="E1159" s="1">
-        <v>43037002</v>
+        <v>41082007</v>
       </c>
       <c r="F1159" s="4">
-        <v>44386.635416666664</v>
+        <v>44386.677083333336</v>
       </c>
       <c r="G1159" s="1" t="s">
         <v>39</v>
@@ -42413,22 +42417,22 @@
     </row>
     <row r="1160" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1160" s="1" t="s">
-        <v>276</v>
+        <v>51</v>
       </c>
       <c r="B1160" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1160" s="1" t="s">
-        <v>1388</v>
+        <v>1214</v>
       </c>
       <c r="D1160" s="1" t="s">
-        <v>1389</v>
+        <v>1213</v>
       </c>
       <c r="E1160" s="1">
-        <v>43037001</v>
+        <v>41082010</v>
       </c>
       <c r="F1160" s="4">
-        <v>44386.552083333336</v>
+        <v>44386.677083333336</v>
       </c>
       <c r="G1160" s="1" t="s">
         <v>39</v>
@@ -42469,22 +42473,22 @@
     </row>
     <row r="1162" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1162" s="1" t="s">
-        <v>276</v>
+        <v>51</v>
       </c>
       <c r="B1162" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1162" s="1" t="s">
-        <v>1391</v>
+        <v>1227</v>
       </c>
       <c r="D1162" s="1" t="s">
-        <v>1391</v>
+        <v>1226</v>
       </c>
       <c r="E1162" s="1">
-        <v>8899004</v>
+        <v>41082009</v>
       </c>
       <c r="F1162" s="4">
-        <v>45093.5625</v>
+        <v>44386.604166666664</v>
       </c>
       <c r="G1162" s="1" t="s">
         <v>39</v>
@@ -42494,7 +42498,7 @@
         <v>23</v>
       </c>
       <c r="J1162" s="1" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="K1162" s="1"/>
       <c r="L1162" s="1"/>
@@ -42502,22 +42506,22 @@
     </row>
     <row r="1163" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1163" s="1" t="s">
-        <v>276</v>
+        <v>51</v>
       </c>
       <c r="B1163" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1163" s="1" t="s">
-        <v>1392</v>
+        <v>1229</v>
       </c>
       <c r="D1163" s="1" t="s">
-        <v>1391</v>
+        <v>1228</v>
       </c>
       <c r="E1163" s="1">
-        <v>43037003</v>
+        <v>41082011</v>
       </c>
       <c r="F1163" s="4">
-        <v>44386.583333333336</v>
+        <v>44385.385416666664</v>
       </c>
       <c r="G1163" s="1" t="s">
         <v>39</v>
@@ -43351,22 +43355,22 @@
     </row>
     <row r="1192" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1192" s="1" t="s">
-        <v>2203</v>
+        <v>276</v>
       </c>
       <c r="B1192" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1192" s="1" t="s">
-        <v>1423</v>
+        <v>1387</v>
       </c>
       <c r="D1192" s="1" t="s">
-        <v>1423</v>
+        <v>1386</v>
       </c>
       <c r="E1192" s="1">
-        <v>8808037</v>
+        <v>43037002</v>
       </c>
       <c r="F1192" s="4">
-        <v>45093.666666666664</v>
+        <v>44386.635416666664</v>
       </c>
       <c r="G1192" s="1" t="s">
         <v>39</v>
@@ -43384,22 +43388,22 @@
     </row>
     <row r="1193" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1193" s="1" t="s">
-        <v>2203</v>
+        <v>276</v>
       </c>
       <c r="B1193" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1193" s="1" t="s">
-        <v>1424</v>
+        <v>1388</v>
       </c>
       <c r="D1193" s="1" t="s">
-        <v>1423</v>
+        <v>1389</v>
       </c>
       <c r="E1193" s="1">
-        <v>43006037</v>
+        <v>43037001</v>
       </c>
       <c r="F1193" s="4">
-        <v>44386.65625</v>
+        <v>44386.552083333336</v>
       </c>
       <c r="G1193" s="1" t="s">
         <v>39</v>
@@ -43529,22 +43533,22 @@
     </row>
     <row r="1198" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1198" s="1" t="s">
-        <v>2203</v>
+        <v>276</v>
       </c>
       <c r="B1198" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1198" s="1" t="s">
-        <v>1429</v>
+        <v>1392</v>
       </c>
       <c r="D1198" s="1" t="s">
-        <v>1429</v>
+        <v>1391</v>
       </c>
       <c r="E1198" s="1">
-        <v>8808013</v>
+        <v>43037003</v>
       </c>
       <c r="F1198" s="4">
-        <v>45093.625</v>
+        <v>44386.583333333336</v>
       </c>
       <c r="G1198" s="1" t="s">
         <v>39</v>
@@ -43554,7 +43558,7 @@
         <v>23</v>
       </c>
       <c r="J1198" s="1" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="K1198" s="1"/>
       <c r="L1198" s="1"/>
@@ -43568,16 +43572,16 @@
         <v>37</v>
       </c>
       <c r="C1199" s="1" t="s">
-        <v>1430</v>
+        <v>1424</v>
       </c>
       <c r="D1199" s="1" t="s">
-        <v>1429</v>
+        <v>1423</v>
       </c>
       <c r="E1199" s="1">
-        <v>43006013</v>
+        <v>43006037</v>
       </c>
       <c r="F1199" s="4">
-        <v>44386.645833333336</v>
+        <v>44386.65625</v>
       </c>
       <c r="G1199" s="1" t="s">
         <v>39</v>
@@ -45110,16 +45114,16 @@
         <v>37</v>
       </c>
       <c r="C1251" s="1" t="s">
-        <v>1484</v>
+        <v>1430</v>
       </c>
       <c r="D1251" s="1" t="s">
-        <v>1484</v>
+        <v>1429</v>
       </c>
       <c r="E1251" s="1">
-        <v>8808038</v>
+        <v>43006013</v>
       </c>
       <c r="F1251" s="4">
-        <v>45093.416666666664</v>
+        <v>44386.645833333336</v>
       </c>
       <c r="G1251" s="1" t="s">
         <v>39</v>
@@ -63487,27 +63491,288 @@
       <c r="M1864" s="1"/>
     </row>
     <row r="1865" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1865" s="1"/>
-      <c r="B1865" s="1"/>
-      <c r="C1865" s="1"/>
+      <c r="A1865" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1865" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1865" t="s">
+        <v>2209</v>
+      </c>
       <c r="D1865" s="1"/>
-      <c r="E1865" s="1"/>
+      <c r="E1865">
+        <v>8934003</v>
+      </c>
       <c r="F1865" s="1"/>
-      <c r="G1865" s="1"/>
+      <c r="G1865" s="1" t="s">
+        <v>426</v>
+      </c>
       <c r="H1865" s="1"/>
-      <c r="I1865" s="1"/>
-      <c r="J1865" s="1"/>
+      <c r="I1865" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1865" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K1865" s="1"/>
       <c r="L1865" s="1"/>
       <c r="M1865" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1864"/>
+  <autoFilter ref="A1:M1865"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1484</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LMS_Mappings xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
+    <Math_Settings xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
+    <Members xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Members>
+    <Has_Leaders_Only_SectionGroup xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
+    <Owner xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Distribution_Groups xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Invited_Leaders xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
+    <NotebookType xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
+    <Leaders xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Leaders>
+    <TeamsChannelId xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
+    <Templates xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
+    <FolderType xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
+    <TaxCatchAll xmlns="b8c1f162-0a68-46db-9c3c-f064fae845ee" xsi:nil="true"/>
+    <Invited_Members xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
+    <CultureName xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
+    <AppVersion xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
+    <Member_Groups xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Member_Groups>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A0B2F798C6660A47A352DEEEB6D87495" ma:contentTypeVersion="36" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aa687342e70d9e845988151f01f819eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="47376c23-eac2-429c-9bcd-0a10e6d6196a" xmlns:ns3="b8c1f162-0a68-46db-9c3c-f064fae845ee" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="539fd4dfa48c38bde8894b72173c8f05" ns2:_="" ns3:_="">
     <xsd:import namespace="47376c23-eac2-429c-9bcd-0a10e6d6196a"/>
@@ -63938,71 +64203,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3604586-D566-4101-9ABE-0E39D593D406}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="47376c23-eac2-429c-9bcd-0a10e6d6196a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b8c1f162-0a68-46db-9c3c-f064fae845ee"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LMS_Mappings xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
-    <Math_Settings xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
-    <Members xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Members>
-    <Has_Leaders_Only_SectionGroup xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
-    <Owner xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Distribution_Groups xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Invited_Leaders xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
-    <NotebookType xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
-    <Leaders xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Leaders>
-    <TeamsChannelId xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
-    <Templates xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
-    <FolderType xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
-    <TaxCatchAll xmlns="b8c1f162-0a68-46db-9c3c-f064fae845ee" xsi:nil="true"/>
-    <Invited_Members xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
-    <CultureName xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
-    <AppVersion xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a" xsi:nil="true"/>
-    <Member_Groups xmlns="47376c23-eac2-429c-9bcd-0a10e6d6196a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Member_Groups>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9D0ED26-8C90-4CF2-8B75-72F468D0C393}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7980BDA-188E-4878-AD73-2DC946C26428}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -64019,29 +64245,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9D0ED26-8C90-4CF2-8B75-72F468D0C393}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3604586-D566-4101-9ABE-0E39D593D406}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="47376c23-eac2-429c-9bcd-0a10e6d6196a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b8c1f162-0a68-46db-9c3c-f064fae845ee"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated master department mapping
</commit_message>
<xml_diff>
--- a/master_amb_mapping_updated.xlsx
+++ b/master_amb_mapping_updated.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$1865</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$1868</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10774" uniqueCount="2210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10754" uniqueCount="2214">
   <si>
     <t>CAMPUS</t>
   </si>
@@ -6658,13 +6658,25 @@
   </si>
   <si>
     <t>4982 HYLAN BLVD THORACIC SURGERY</t>
+  </si>
+  <si>
+    <t>MSSN</t>
+  </si>
+  <si>
+    <t>242 MERRICK RD NEUROSURGERY</t>
+  </si>
+  <si>
+    <t>3131 KINGS HIGHWAY NEUROSURGERY</t>
+  </si>
+  <si>
+    <t>5 CUBA HILL NEUROSURGERY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6687,8 +6699,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6707,6 +6726,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -6720,12 +6745,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="22" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7006,22 +7037,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1865"/>
+  <dimension ref="A1:M1868"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C1878" sqref="C1877:C1878"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.85546875" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="53.42578125" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="36.7109375" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.28515625" customWidth="1"/>
@@ -7360,9 +7391,7 @@
       <c r="F12" s="4">
         <v>45086.479166666664</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -8932,62 +8961,60 @@
     </row>
     <row r="61" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>2200</v>
+        <v>12</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>521</v>
+        <v>37</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="E61" s="1">
-        <v>8011005</v>
+        <v>8938010</v>
       </c>
       <c r="F61" s="4">
-        <v>45093.680555555555</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>45090.458333333336</v>
+      </c>
+      <c r="G61" s="1"/>
       <c r="H61" s="1"/>
-      <c r="I61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
     </row>
     <row r="62" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>2202</v>
+        <v>2200</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>37</v>
+        <v>521</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>109</v>
+        <v>522</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>108</v>
+        <v>522</v>
       </c>
       <c r="E62" s="1">
-        <v>41001042</v>
+        <v>8011005</v>
       </c>
       <c r="F62" s="4">
-        <v>44292.5</v>
+        <v>45093.680555555555</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
+      <c r="I62" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
@@ -11434,34 +11461,26 @@
       <c r="M137" s="1"/>
     </row>
     <row r="138" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
-        <v>2200</v>
-      </c>
+      <c r="A138" s="1"/>
       <c r="B138" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>680</v>
+        <v>631</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>680</v>
+        <v>631</v>
       </c>
       <c r="E138" s="1">
-        <v>8004026</v>
+        <v>8614002</v>
       </c>
       <c r="F138" s="4">
-        <v>45093.375</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>45083.291666666664</v>
+      </c>
+      <c r="G138" s="1"/>
       <c r="H138" s="1"/>
-      <c r="I138" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J138" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="I138" s="1"/>
+      <c r="J138" s="1"/>
       <c r="K138" s="1"/>
       <c r="L138" s="1"/>
       <c r="M138" s="1"/>
@@ -12140,16 +12159,16 @@
         <v>248</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="E159" s="1">
-        <v>41001035</v>
+        <v>8823009</v>
       </c>
       <c r="F159" s="4">
-        <v>44386.645833333336</v>
+        <v>45093.583333333336</v>
       </c>
       <c r="G159" s="1" t="s">
         <v>248</v>
@@ -12276,16 +12295,16 @@
         <v>248</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E163" s="1">
-        <v>8823009</v>
+        <v>8823013</v>
       </c>
       <c r="F163" s="4">
-        <v>45093.583333333336</v>
+        <v>45093.479166666664</v>
       </c>
       <c r="G163" s="1" t="s">
         <v>248</v>
@@ -12309,16 +12328,16 @@
         <v>248</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="E164" s="1">
-        <v>41001033</v>
+        <v>8823012</v>
       </c>
       <c r="F164" s="4">
-        <v>44386.6875</v>
+        <v>45093.583333333336</v>
       </c>
       <c r="G164" s="1" t="s">
         <v>248</v>
@@ -12336,22 +12355,22 @@
     </row>
     <row r="165" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>2202</v>
+        <v>276</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>256</v>
+        <v>319</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>256</v>
+        <v>319</v>
       </c>
       <c r="E165" s="1">
-        <v>8823013</v>
+        <v>8503001</v>
       </c>
       <c r="F165" s="4">
-        <v>45093.479166666664</v>
+        <v>45093.666666666664</v>
       </c>
       <c r="G165" s="1" t="s">
         <v>248</v>
@@ -12369,22 +12388,22 @@
     </row>
     <row r="166" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>2202</v>
+        <v>276</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>257</v>
+        <v>321</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>256</v>
+        <v>321</v>
       </c>
       <c r="E166" s="1">
-        <v>41001037</v>
+        <v>8802045</v>
       </c>
       <c r="F166" s="4">
-        <v>44385.666666666664</v>
+        <v>45093.604166666664</v>
       </c>
       <c r="G166" s="1" t="s">
         <v>248</v>
@@ -12534,22 +12553,22 @@
     </row>
     <row r="171" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>2202</v>
+        <v>2203</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>263</v>
+        <v>435</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>263</v>
+        <v>435</v>
       </c>
       <c r="E171" s="1">
-        <v>8823012</v>
+        <v>8803007</v>
       </c>
       <c r="F171" s="4">
-        <v>45093.583333333336</v>
+        <v>45093.625</v>
       </c>
       <c r="G171" s="1" t="s">
         <v>248</v>
@@ -12567,22 +12586,22 @@
     </row>
     <row r="172" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>2202</v>
+        <v>16</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>264</v>
+        <v>603</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>263</v>
+        <v>603</v>
       </c>
       <c r="E172" s="1">
-        <v>41001036</v>
+        <v>8052002</v>
       </c>
       <c r="F172" s="4">
-        <v>44385.6875</v>
+        <v>45092.645833333336</v>
       </c>
       <c r="G172" s="1" t="s">
         <v>248</v>
@@ -13600,56 +13619,50 @@
       <c r="M205" s="1"/>
     </row>
     <row r="206" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="1" t="s">
-        <v>2200</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C206" s="1" t="s">
-        <v>695</v>
+      <c r="A206" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="C206" s="5" t="s">
+        <v>643</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>695</v>
-      </c>
-      <c r="E206" s="1">
-        <v>8005002</v>
-      </c>
-      <c r="F206" s="4">
-        <v>45096.645833333336</v>
-      </c>
-      <c r="G206" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H206" s="1"/>
-      <c r="I206" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J206" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>643</v>
+      </c>
+      <c r="E206" s="5">
+        <v>8004015</v>
+      </c>
+      <c r="F206" s="6">
+        <v>44980.604166666664</v>
+      </c>
+      <c r="G206" s="5"/>
+      <c r="H206" s="5"/>
+      <c r="I206" s="5"/>
+      <c r="J206" s="5"/>
       <c r="K206" s="1"/>
       <c r="L206" s="1"/>
       <c r="M206" s="1"/>
     </row>
     <row r="207" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>12</v>
+        <v>2200</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>1147</v>
+        <v>680</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>1147</v>
+        <v>680</v>
       </c>
       <c r="E207" s="1">
-        <v>8811002</v>
+        <v>8004026</v>
       </c>
       <c r="F207" s="4">
-        <v>45093.625</v>
+        <v>45093.375</v>
       </c>
       <c r="G207" s="1" t="s">
         <v>39</v>
@@ -13845,22 +13858,22 @@
     </row>
     <row r="214" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>276</v>
+        <v>2200</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>319</v>
+        <v>665</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>319</v>
+        <v>665</v>
       </c>
       <c r="E214" s="1">
-        <v>8503001</v>
+        <v>8004059</v>
       </c>
       <c r="F214" s="4">
-        <v>45093.666666666664</v>
+        <v>45092.604166666664</v>
       </c>
       <c r="G214" s="1" t="s">
         <v>248</v>
@@ -13878,22 +13891,22 @@
     </row>
     <row r="215" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>276</v>
+        <v>2200</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>320</v>
+        <v>684</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>319</v>
+        <v>684</v>
       </c>
       <c r="E215" s="1">
-        <v>43001049</v>
+        <v>8004035</v>
       </c>
       <c r="F215" s="4">
-        <v>44386.625</v>
+        <v>45093.729166666664</v>
       </c>
       <c r="G215" s="1" t="s">
         <v>248</v>
@@ -13911,22 +13924,22 @@
     </row>
     <row r="216" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>276</v>
+        <v>51</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>321</v>
+        <v>1134</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>321</v>
+        <v>1134</v>
       </c>
       <c r="E216" s="1">
-        <v>8802045</v>
+        <v>8811010</v>
       </c>
       <c r="F216" s="4">
-        <v>45093.604166666664</v>
+        <v>45091.645833333336</v>
       </c>
       <c r="G216" s="1" t="s">
         <v>248</v>
@@ -13944,22 +13957,22 @@
     </row>
     <row r="217" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>276</v>
+        <v>16</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>322</v>
+        <v>1587</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>321</v>
+        <v>1587</v>
       </c>
       <c r="E217" s="1">
-        <v>43001046</v>
+        <v>8001032</v>
       </c>
       <c r="F217" s="4">
-        <v>44386.708333333336</v>
+        <v>45094.645833333336</v>
       </c>
       <c r="G217" s="1" t="s">
         <v>248</v>
@@ -16672,22 +16685,22 @@
     </row>
     <row r="309" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
-        <v>2203</v>
+        <v>16</v>
       </c>
       <c r="B309" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>435</v>
+        <v>1588</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>435</v>
+        <v>1588</v>
       </c>
       <c r="E309" s="1">
-        <v>8803007</v>
+        <v>8001031</v>
       </c>
       <c r="F309" s="4">
-        <v>45093.625</v>
+        <v>45093.583333333336</v>
       </c>
       <c r="G309" s="1" t="s">
         <v>248</v>
@@ -16705,22 +16718,22 @@
     </row>
     <row r="310" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
-        <v>2203</v>
+        <v>16</v>
       </c>
       <c r="B310" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>436</v>
+        <v>1589</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>435</v>
+        <v>1589</v>
       </c>
       <c r="E310" s="1">
-        <v>43002007</v>
+        <v>8001030</v>
       </c>
       <c r="F310" s="4">
-        <v>44385.583333333336</v>
+        <v>45094.666666666664</v>
       </c>
       <c r="G310" s="1" t="s">
         <v>248</v>
@@ -18638,7 +18651,7 @@
       </c>
       <c r="H373" s="1"/>
       <c r="I373" s="1" t="s">
-        <v>475</v>
+        <v>23</v>
       </c>
       <c r="J373" s="1" t="s">
         <v>24</v>
@@ -18678,29 +18691,35 @@
     </row>
     <row r="375" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>37</v>
+        <v>681</v>
       </c>
       <c r="C375" s="1" t="s">
-        <v>509</v>
+        <v>682</v>
       </c>
       <c r="D375" s="1" t="s">
-        <v>509</v>
+        <v>682</v>
       </c>
       <c r="E375" s="1">
-        <v>8938010</v>
+        <v>8004023</v>
       </c>
       <c r="F375" s="4">
-        <v>45090.458333333336</v>
+        <v>45093.666666666664</v>
       </c>
       <c r="G375" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H375" s="1"/>
-      <c r="I375" s="1"/>
-      <c r="J375" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="H375" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="I375" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J375" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K375" s="1"/>
       <c r="L375" s="1"/>
       <c r="M375" s="1"/>
@@ -19013,22 +19032,22 @@
     </row>
     <row r="386" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>51</v>
+        <v>2200</v>
       </c>
       <c r="B386" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C386" s="1" t="s">
-        <v>1207</v>
+        <v>695</v>
       </c>
       <c r="D386" s="1" t="s">
-        <v>1207</v>
+        <v>695</v>
       </c>
       <c r="E386" s="1">
-        <v>8881007</v>
+        <v>8005002</v>
       </c>
       <c r="F386" s="4">
-        <v>45093.6875</v>
+        <v>45096.645833333336</v>
       </c>
       <c r="G386" s="1" t="s">
         <v>39</v>
@@ -19045,34 +19064,26 @@
       <c r="M386" s="1"/>
     </row>
     <row r="387" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A387" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="A387" s="1"/>
       <c r="B387" s="1" t="s">
-        <v>37</v>
+        <v>642</v>
       </c>
       <c r="C387" s="1" t="s">
-        <v>1209</v>
+        <v>762</v>
       </c>
       <c r="D387" s="1" t="s">
-        <v>1209</v>
+        <v>762</v>
       </c>
       <c r="E387" s="1">
-        <v>8881008</v>
+        <v>80020111</v>
       </c>
       <c r="F387" s="4">
-        <v>45093.666666666664</v>
-      </c>
-      <c r="G387" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>45093.583333333336</v>
+      </c>
+      <c r="G387" s="1"/>
       <c r="H387" s="1"/>
-      <c r="I387" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J387" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="I387" s="1"/>
+      <c r="J387" s="1"/>
       <c r="K387" s="1"/>
       <c r="L387" s="1"/>
       <c r="M387" s="1"/>
@@ -21202,19 +21213,19 @@
         <v>16</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>248</v>
+        <v>505</v>
       </c>
       <c r="C458" s="1" t="s">
-        <v>603</v>
+        <v>1608</v>
       </c>
       <c r="D458" s="1" t="s">
-        <v>603</v>
+        <v>1608</v>
       </c>
       <c r="E458" s="1">
-        <v>8052002</v>
+        <v>8001021</v>
       </c>
       <c r="F458" s="4">
-        <v>45092.645833333336</v>
+        <v>45093.645833333336</v>
       </c>
       <c r="G458" s="1" t="s">
         <v>248</v>
@@ -21910,21 +21921,23 @@
       <c r="M481" s="1"/>
     </row>
     <row r="482" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A482" s="1"/>
+      <c r="A482" s="1" t="s">
+        <v>2200</v>
+      </c>
       <c r="B482" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C482" s="1" t="s">
-        <v>631</v>
+        <v>768</v>
       </c>
       <c r="D482" s="1" t="s">
-        <v>631</v>
+        <v>768</v>
       </c>
       <c r="E482" s="1">
-        <v>8614002</v>
+        <v>8366002</v>
       </c>
       <c r="F482" s="4">
-        <v>45083.291666666664</v>
+        <v>45093.479166666664</v>
       </c>
       <c r="G482" s="1"/>
       <c r="H482" s="1"/>
@@ -22244,26 +22257,24 @@
     </row>
     <row r="493" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A493" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>642</v>
+        <v>37</v>
       </c>
       <c r="C493" s="1" t="s">
-        <v>643</v>
+        <v>968</v>
       </c>
       <c r="D493" s="1" t="s">
-        <v>643</v>
+        <v>968</v>
       </c>
       <c r="E493" s="1">
-        <v>8004015</v>
+        <v>8800003</v>
       </c>
       <c r="F493" s="4">
-        <v>44980.604166666664</v>
-      </c>
-      <c r="G493" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>45093.59375</v>
+      </c>
+      <c r="G493" s="1"/>
       <c r="H493" s="1"/>
       <c r="I493" s="1"/>
       <c r="J493" s="1"/>
@@ -22808,22 +22819,22 @@
     </row>
     <row r="511" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A511" s="1" t="s">
-        <v>2200</v>
+        <v>16</v>
       </c>
       <c r="B511" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C511" s="1" t="s">
-        <v>665</v>
+        <v>1637</v>
       </c>
       <c r="D511" s="1" t="s">
-        <v>665</v>
+        <v>1637</v>
       </c>
       <c r="E511" s="1">
-        <v>8004059</v>
+        <v>8001088</v>
       </c>
       <c r="F511" s="4">
-        <v>45092.604166666664</v>
+        <v>45092.458333333336</v>
       </c>
       <c r="G511" s="1" t="s">
         <v>248</v>
@@ -23151,68 +23162,54 @@
     </row>
     <row r="522" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A522" s="1" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B522" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C522" s="1" t="s">
-        <v>1213</v>
+        <v>971</v>
       </c>
       <c r="D522" s="1" t="s">
-        <v>1213</v>
+        <v>971</v>
       </c>
       <c r="E522" s="1">
-        <v>8881010</v>
+        <v>8800009</v>
       </c>
       <c r="F522" s="4">
         <v>45093.625</v>
       </c>
-      <c r="G522" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="G522" s="1"/>
       <c r="H522" s="1"/>
-      <c r="I522" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J522" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="I522" s="1"/>
+      <c r="J522" s="1"/>
       <c r="K522" s="1"/>
       <c r="L522" s="1"/>
       <c r="M522" s="1"/>
     </row>
     <row r="523" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A523" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B523" s="1" t="s">
-        <v>681</v>
-      </c>
-      <c r="C523" s="1" t="s">
-        <v>682</v>
+      <c r="A523" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B523" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C523" s="5" t="s">
+        <v>1123</v>
       </c>
       <c r="D523" s="1" t="s">
-        <v>682</v>
-      </c>
-      <c r="E523" s="1">
-        <v>8004023</v>
-      </c>
-      <c r="F523" s="4">
-        <v>45093.666666666664</v>
-      </c>
-      <c r="G523" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="H523" s="1" t="s">
-        <v>642</v>
-      </c>
-      <c r="I523" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J523" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>1123</v>
+      </c>
+      <c r="E523" s="5">
+        <v>8811001</v>
+      </c>
+      <c r="F523" s="6">
+        <v>45093.6875</v>
+      </c>
+      <c r="G523" s="5"/>
+      <c r="H523" s="5"/>
+      <c r="I523" s="5"/>
+      <c r="J523" s="5"/>
       <c r="K523" s="1"/>
       <c r="L523" s="1"/>
       <c r="M523" s="1"/>
@@ -23254,22 +23251,22 @@
     </row>
     <row r="525" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A525" s="1" t="s">
-        <v>2200</v>
+        <v>16</v>
       </c>
       <c r="B525" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C525" s="1" t="s">
-        <v>684</v>
+        <v>1638</v>
       </c>
       <c r="D525" s="1" t="s">
-        <v>684</v>
+        <v>1638</v>
       </c>
       <c r="E525" s="1">
-        <v>8004035</v>
+        <v>8001084</v>
       </c>
       <c r="F525" s="4">
-        <v>45093.729166666664</v>
+        <v>45084.666666666664</v>
       </c>
       <c r="G525" s="1" t="s">
         <v>248</v>
@@ -23583,34 +23580,28 @@
       <c r="M534" s="1"/>
     </row>
     <row r="535" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A535" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B535" s="1" t="s">
+      <c r="A535" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B535" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C535" s="1" t="s">
-        <v>1226</v>
+      <c r="C535" s="5" t="s">
+        <v>1129</v>
       </c>
       <c r="D535" s="1" t="s">
-        <v>1226</v>
-      </c>
-      <c r="E535" s="1">
-        <v>8881009</v>
-      </c>
-      <c r="F535" s="4">
-        <v>45000.354166666664</v>
-      </c>
-      <c r="G535" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H535" s="1"/>
-      <c r="I535" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J535" s="1" t="s">
-        <v>112</v>
-      </c>
+        <v>1129</v>
+      </c>
+      <c r="E535" s="5">
+        <v>8811011</v>
+      </c>
+      <c r="F535" s="6">
+        <v>45085.479166666664</v>
+      </c>
+      <c r="G535" s="5"/>
+      <c r="H535" s="5"/>
+      <c r="I535" s="5"/>
+      <c r="J535" s="5"/>
       <c r="K535" s="1"/>
       <c r="L535" s="1"/>
       <c r="M535" s="1"/>
@@ -25275,16 +25266,10 @@
       <c r="F589" s="4">
         <v>45091.645833333336</v>
       </c>
-      <c r="G589" s="1" t="s">
-        <v>122</v>
-      </c>
+      <c r="G589" s="1"/>
       <c r="H589" s="1"/>
-      <c r="I589" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J589" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="I589" s="1"/>
+      <c r="J589" s="1"/>
       <c r="K589" s="1"/>
       <c r="L589" s="1"/>
       <c r="M589" s="1"/>
@@ -25476,28 +25461,34 @@
       <c r="M595" s="1"/>
     </row>
     <row r="596" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A596" s="1"/>
+      <c r="A596" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B596" s="1" t="s">
-        <v>642</v>
+        <v>37</v>
       </c>
       <c r="C596" s="1" t="s">
-        <v>762</v>
+        <v>1147</v>
       </c>
       <c r="D596" s="1" t="s">
-        <v>762</v>
+        <v>1147</v>
       </c>
       <c r="E596" s="1">
-        <v>80020111</v>
+        <v>8811002</v>
       </c>
       <c r="F596" s="4">
-        <v>45093.583333333336</v>
+        <v>45093.625</v>
       </c>
       <c r="G596" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H596" s="1"/>
-      <c r="I596" s="1"/>
-      <c r="J596" s="1"/>
+      <c r="I596" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J596" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K596" s="1"/>
       <c r="L596" s="1"/>
       <c r="M596" s="1"/>
@@ -25637,30 +25628,28 @@
       <c r="M600" s="1"/>
     </row>
     <row r="601" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A601" s="1" t="s">
-        <v>2200</v>
-      </c>
-      <c r="B601" s="1" t="s">
+      <c r="A601" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B601" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C601" s="1" t="s">
-        <v>768</v>
+      <c r="C601" s="5" t="s">
+        <v>1149</v>
       </c>
       <c r="D601" s="1" t="s">
-        <v>768</v>
-      </c>
-      <c r="E601" s="1">
-        <v>8366002</v>
-      </c>
-      <c r="F601" s="4">
-        <v>45093.479166666664</v>
-      </c>
-      <c r="G601" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H601" s="1"/>
-      <c r="I601" s="1"/>
-      <c r="J601" s="1"/>
+        <v>1149</v>
+      </c>
+      <c r="E601" s="5">
+        <v>8811003</v>
+      </c>
+      <c r="F601" s="6">
+        <v>45093.354166666664</v>
+      </c>
+      <c r="G601" s="5"/>
+      <c r="H601" s="5"/>
+      <c r="I601" s="5"/>
+      <c r="J601" s="5"/>
       <c r="K601" s="1"/>
       <c r="L601" s="1"/>
       <c r="M601" s="1"/>
@@ -30853,87 +30842,99 @@
     </row>
     <row r="778" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A778" s="1" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B778" s="1" t="s">
-        <v>37</v>
+        <v>521</v>
       </c>
       <c r="C778" s="1" t="s">
-        <v>968</v>
+        <v>1195</v>
       </c>
       <c r="D778" s="1" t="s">
-        <v>968</v>
+        <v>1195</v>
       </c>
       <c r="E778" s="1">
-        <v>8800003</v>
+        <v>8881006</v>
       </c>
       <c r="F778" s="4">
-        <v>45093.59375</v>
+        <v>45093.614583333336</v>
       </c>
       <c r="G778" s="1" t="s">
-        <v>39</v>
+        <v>202</v>
       </c>
       <c r="H778" s="1"/>
-      <c r="I778" s="1"/>
-      <c r="J778" s="1"/>
+      <c r="I778" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J778" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K778" s="1"/>
       <c r="L778" s="1"/>
       <c r="M778" s="1"/>
     </row>
     <row r="779" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A779" s="1" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B779" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C779" s="1" t="s">
-        <v>969</v>
+        <v>1207</v>
       </c>
       <c r="D779" s="1" t="s">
-        <v>970</v>
+        <v>1207</v>
       </c>
       <c r="E779" s="1">
-        <v>8800004</v>
+        <v>8881007</v>
       </c>
       <c r="F779" s="4">
-        <v>44771.354166666664</v>
+        <v>45093.6875</v>
       </c>
       <c r="G779" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H779" s="1"/>
-      <c r="I779" s="1"/>
-      <c r="J779" s="1"/>
+      <c r="I779" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J779" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K779" s="1"/>
       <c r="L779" s="1"/>
       <c r="M779" s="1"/>
     </row>
     <row r="780" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A780" s="1" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B780" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C780" s="1" t="s">
-        <v>971</v>
+        <v>1209</v>
       </c>
       <c r="D780" s="1" t="s">
-        <v>971</v>
+        <v>1209</v>
       </c>
       <c r="E780" s="1">
-        <v>8800009</v>
+        <v>8881008</v>
       </c>
       <c r="F780" s="4">
-        <v>45093.625</v>
+        <v>45093.666666666664</v>
       </c>
       <c r="G780" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H780" s="1"/>
-      <c r="I780" s="1"/>
-      <c r="J780" s="1"/>
+      <c r="I780" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J780" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="K780" s="1"/>
       <c r="L780" s="1"/>
       <c r="M780" s="1"/>
@@ -31134,7 +31135,7 @@
       </c>
       <c r="H787" s="1"/>
       <c r="I787" s="1" t="s">
-        <v>475</v>
+        <v>23</v>
       </c>
       <c r="J787" s="1" t="s">
         <v>24</v>
@@ -31479,29 +31480,33 @@
     </row>
     <row r="800" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A800" s="1" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B800" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C800" s="1" t="s">
-        <v>993</v>
+        <v>1213</v>
       </c>
       <c r="D800" s="1" t="s">
-        <v>994</v>
+        <v>1213</v>
       </c>
       <c r="E800" s="1">
-        <v>8800005</v>
+        <v>8881010</v>
       </c>
       <c r="F800" s="4">
-        <v>44771.625</v>
+        <v>45093.625</v>
       </c>
       <c r="G800" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H800" s="1"/>
-      <c r="I800" s="1"/>
-      <c r="J800" s="1"/>
+      <c r="I800" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J800" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="K800" s="1"/>
       <c r="L800" s="1"/>
       <c r="M800" s="1"/>
@@ -32042,58 +32047,66 @@
     </row>
     <row r="819" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A819" s="1" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B819" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C819" s="1" t="s">
-        <v>1016</v>
+        <v>1226</v>
       </c>
       <c r="D819" s="1" t="s">
-        <v>1017</v>
+        <v>1226</v>
       </c>
       <c r="E819" s="1">
-        <v>8913002</v>
+        <v>8881009</v>
       </c>
       <c r="F819" s="4">
-        <v>44396.625</v>
+        <v>45000.354166666664</v>
       </c>
       <c r="G819" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H819" s="1"/>
-      <c r="I819" s="1"/>
-      <c r="J819" s="1"/>
+      <c r="I819" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J819" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="K819" s="1"/>
       <c r="L819" s="1"/>
       <c r="M819" s="1"/>
     </row>
     <row r="820" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A820" s="1" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B820" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C820" s="1" t="s">
-        <v>1018</v>
+        <v>1228</v>
       </c>
       <c r="D820" s="1" t="s">
-        <v>1019</v>
+        <v>1228</v>
       </c>
       <c r="E820" s="1">
-        <v>8913003</v>
+        <v>8881011</v>
       </c>
       <c r="F820" s="4">
-        <v>44396.666666666664</v>
+        <v>44862.541666666664</v>
       </c>
       <c r="G820" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H820" s="1"/>
-      <c r="I820" s="1"/>
-      <c r="J820" s="1"/>
+      <c r="I820" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J820" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="K820" s="1"/>
       <c r="L820" s="1"/>
       <c r="M820" s="1"/>
@@ -32106,20 +32119,18 @@
         <v>37</v>
       </c>
       <c r="C821" s="1" t="s">
-        <v>1020</v>
+        <v>1285</v>
       </c>
       <c r="D821" s="1" t="s">
-        <v>1021</v>
+        <v>1285</v>
       </c>
       <c r="E821" s="1">
-        <v>8913001</v>
+        <v>8348010</v>
       </c>
       <c r="F821" s="4">
-        <v>44396.5</v>
-      </c>
-      <c r="G821" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>45012.520833333336</v>
+      </c>
+      <c r="G821" s="1"/>
       <c r="H821" s="1"/>
       <c r="I821" s="1"/>
       <c r="J821" s="1"/>
@@ -34869,58 +34880,60 @@
     </row>
     <row r="914" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A914" s="1" t="s">
-        <v>12</v>
+        <v>276</v>
       </c>
       <c r="B914" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C914" s="1" t="s">
-        <v>1123</v>
+        <v>1366</v>
       </c>
       <c r="D914" s="1" t="s">
-        <v>1123</v>
+        <v>1366</v>
       </c>
       <c r="E914" s="1">
-        <v>8811001</v>
+        <v>8805016</v>
       </c>
       <c r="F914" s="4">
-        <v>45093.6875</v>
+        <v>45093.635416666664</v>
       </c>
       <c r="G914" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H914" s="1"/>
-      <c r="I914" s="1"/>
-      <c r="J914" s="1"/>
+      <c r="I914" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J914" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K914" s="1"/>
       <c r="L914" s="1"/>
       <c r="M914" s="1"/>
     </row>
     <row r="915" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A915" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B915" s="1" t="s">
+      <c r="A915" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B915" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C915" s="1" t="s">
-        <v>1124</v>
+      <c r="C915" s="5" t="s">
+        <v>1376</v>
       </c>
       <c r="D915" s="1" t="s">
-        <v>1123</v>
-      </c>
-      <c r="E915" s="1">
-        <v>41002001</v>
-      </c>
-      <c r="F915" s="4">
-        <v>44386.684027777781</v>
-      </c>
-      <c r="G915" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H915" s="1"/>
-      <c r="I915" s="1"/>
-      <c r="J915" s="1"/>
+        <v>1376</v>
+      </c>
+      <c r="E915" s="5">
+        <v>8805032</v>
+      </c>
+      <c r="F915" s="6">
+        <v>45093.541666666664</v>
+      </c>
+      <c r="G915" s="5"/>
+      <c r="H915" s="5"/>
+      <c r="I915" s="5"/>
+      <c r="J915" s="5"/>
       <c r="K915" s="1"/>
       <c r="L915" s="1"/>
       <c r="M915" s="1"/>
@@ -35051,58 +35064,56 @@
     </row>
     <row r="920" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A920" s="1" t="s">
-        <v>12</v>
+        <v>276</v>
       </c>
       <c r="B920" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C920" s="1" t="s">
-        <v>1129</v>
+        <v>1386</v>
       </c>
       <c r="D920" s="1" t="s">
-        <v>1129</v>
+        <v>1386</v>
       </c>
       <c r="E920" s="1">
-        <v>8811011</v>
+        <v>8899003</v>
       </c>
       <c r="F920" s="4">
-        <v>45085.479166666664</v>
+        <v>45093.625</v>
       </c>
       <c r="G920" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H920" s="1"/>
-      <c r="I920" s="1"/>
-      <c r="J920" s="1"/>
+      <c r="I920" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J920" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="K920" s="1"/>
       <c r="L920" s="1"/>
       <c r="M920" s="1"/>
     </row>
     <row r="921" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A921" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B921" s="1" t="s">
+      <c r="A921" s="5"/>
+      <c r="B921" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C921" s="1" t="s">
-        <v>1130</v>
+      <c r="C921" s="5" t="s">
+        <v>1390</v>
       </c>
       <c r="D921" s="1" t="s">
-        <v>1129</v>
-      </c>
-      <c r="E921" s="1">
-        <v>41002009</v>
-      </c>
-      <c r="F921" s="4">
-        <v>44386.458333333336</v>
-      </c>
-      <c r="G921" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H921" s="1"/>
-      <c r="I921" s="1"/>
-      <c r="J921" s="1"/>
+        <v>1390</v>
+      </c>
+      <c r="E921" s="5">
+        <v>8899010</v>
+      </c>
+      <c r="F921" s="5"/>
+      <c r="G921" s="5"/>
+      <c r="H921" s="5"/>
+      <c r="I921" s="5"/>
+      <c r="J921" s="5"/>
       <c r="K921" s="1"/>
       <c r="L921" s="1"/>
       <c r="M921" s="1"/>
@@ -35223,22 +35234,22 @@
     </row>
     <row r="926" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A926" s="1" t="s">
-        <v>51</v>
+        <v>2202</v>
       </c>
       <c r="B926" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C926" s="1" t="s">
-        <v>1134</v>
+        <v>250</v>
       </c>
       <c r="D926" s="1" t="s">
-        <v>1134</v>
+        <v>249</v>
       </c>
       <c r="E926" s="1">
-        <v>8811010</v>
+        <v>41001035</v>
       </c>
       <c r="F926" s="4">
-        <v>45091.645833333336</v>
+        <v>44386.645833333336</v>
       </c>
       <c r="G926" s="1" t="s">
         <v>248</v>
@@ -35602,22 +35613,22 @@
     </row>
     <row r="939" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A939" s="1" t="s">
-        <v>51</v>
+        <v>276</v>
       </c>
       <c r="B939" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C939" s="1" t="s">
-        <v>1228</v>
+        <v>1391</v>
       </c>
       <c r="D939" s="1" t="s">
-        <v>1228</v>
+        <v>1391</v>
       </c>
       <c r="E939" s="1">
-        <v>8881011</v>
+        <v>8899004</v>
       </c>
       <c r="F939" s="4">
-        <v>44862.541666666664</v>
+        <v>45093.5625</v>
       </c>
       <c r="G939" s="1" t="s">
         <v>39</v>
@@ -35635,87 +35646,89 @@
     </row>
     <row r="940" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A940" s="1" t="s">
-        <v>12</v>
+        <v>2203</v>
       </c>
       <c r="B940" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C940" s="1" t="s">
-        <v>1148</v>
+        <v>1423</v>
       </c>
       <c r="D940" s="1" t="s">
-        <v>1147</v>
+        <v>1423</v>
       </c>
       <c r="E940" s="1">
-        <v>41002002</v>
+        <v>8808037</v>
       </c>
       <c r="F940" s="4">
-        <v>44386.583333333336</v>
+        <v>45093.666666666664</v>
       </c>
       <c r="G940" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H940" s="1"/>
-      <c r="I940" s="1"/>
-      <c r="J940" s="1"/>
+      <c r="I940" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J940" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K940" s="1"/>
       <c r="L940" s="1"/>
       <c r="M940" s="1"/>
     </row>
     <row r="941" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A941" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B941" s="1" t="s">
+      <c r="A941" s="5"/>
+      <c r="B941" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C941" s="1" t="s">
-        <v>1149</v>
+      <c r="C941" s="5" t="s">
+        <v>1428</v>
       </c>
       <c r="D941" s="1" t="s">
-        <v>1149</v>
-      </c>
-      <c r="E941" s="1">
-        <v>8811003</v>
-      </c>
-      <c r="F941" s="4">
-        <v>45093.354166666664</v>
-      </c>
-      <c r="G941" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H941" s="1"/>
-      <c r="I941" s="1"/>
-      <c r="J941" s="1"/>
+        <v>1428</v>
+      </c>
+      <c r="E941" s="5">
+        <v>8808077</v>
+      </c>
+      <c r="F941" s="5"/>
+      <c r="G941" s="5"/>
+      <c r="H941" s="5"/>
+      <c r="I941" s="5"/>
+      <c r="J941" s="5"/>
       <c r="K941" s="1"/>
       <c r="L941" s="1"/>
       <c r="M941" s="1"/>
     </row>
     <row r="942" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A942" s="1" t="s">
-        <v>12</v>
+        <v>2203</v>
       </c>
       <c r="B942" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C942" s="1" t="s">
-        <v>1150</v>
+        <v>1429</v>
       </c>
       <c r="D942" s="1" t="s">
-        <v>1149</v>
+        <v>1429</v>
       </c>
       <c r="E942" s="1">
-        <v>41002003</v>
+        <v>8808013</v>
       </c>
       <c r="F942" s="4">
-        <v>44385.5625</v>
+        <v>45093.625</v>
       </c>
       <c r="G942" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H942" s="1"/>
-      <c r="I942" s="1"/>
-      <c r="J942" s="1"/>
+      <c r="I942" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J942" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="K942" s="1"/>
       <c r="L942" s="1"/>
       <c r="M942" s="1"/>
@@ -36737,25 +36750,25 @@
     </row>
     <row r="978" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A978" s="1" t="s">
-        <v>51</v>
+        <v>2203</v>
       </c>
       <c r="B978" s="1" t="s">
-        <v>521</v>
+        <v>37</v>
       </c>
       <c r="C978" s="1" t="s">
-        <v>1195</v>
+        <v>1484</v>
       </c>
       <c r="D978" s="1" t="s">
-        <v>1195</v>
+        <v>1484</v>
       </c>
       <c r="E978" s="1">
-        <v>8881006</v>
+        <v>8808038</v>
       </c>
       <c r="F978" s="4">
-        <v>45093.614583333336</v>
+        <v>45093.416666666664</v>
       </c>
       <c r="G978" s="1" t="s">
-        <v>202</v>
+        <v>39</v>
       </c>
       <c r="H978" s="1"/>
       <c r="I978" s="1" t="s">
@@ -36769,34 +36782,28 @@
       <c r="M978" s="1"/>
     </row>
     <row r="979" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A979" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B979" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="C979" s="1" t="s">
-        <v>1196</v>
+      <c r="A979" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B979" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="C979" s="5" t="s">
+        <v>1540</v>
       </c>
       <c r="D979" s="1" t="s">
-        <v>1195</v>
-      </c>
-      <c r="E979" s="1">
-        <v>41082006</v>
-      </c>
-      <c r="F979" s="4">
-        <v>44385.635416666664</v>
-      </c>
-      <c r="G979" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="H979" s="1"/>
-      <c r="I979" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J979" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>1540</v>
+      </c>
+      <c r="E979" s="5">
+        <v>8849007</v>
+      </c>
+      <c r="F979" s="6">
+        <v>45093.6875</v>
+      </c>
+      <c r="G979" s="5"/>
+      <c r="H979" s="5"/>
+      <c r="I979" s="5"/>
+      <c r="J979" s="5"/>
       <c r="K979" s="1"/>
       <c r="L979" s="1"/>
       <c r="M979" s="1"/>
@@ -37068,133 +37075,107 @@
       <c r="M987" s="1"/>
     </row>
     <row r="988" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A988" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B988" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C988" s="1" t="s">
-        <v>1366</v>
+      <c r="A988" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B988" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="C988" s="5" t="s">
+        <v>1585</v>
       </c>
       <c r="D988" s="1" t="s">
-        <v>1366</v>
-      </c>
-      <c r="E988" s="1">
-        <v>8805016</v>
-      </c>
-      <c r="F988" s="4">
-        <v>45093.635416666664</v>
-      </c>
-      <c r="G988" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H988" s="1"/>
-      <c r="I988" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J988" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>1585</v>
+      </c>
+      <c r="E988" s="5">
+        <v>8001061</v>
+      </c>
+      <c r="F988" s="6">
+        <v>45063.5</v>
+      </c>
+      <c r="G988" s="5"/>
+      <c r="H988" s="5"/>
+      <c r="I988" s="5"/>
+      <c r="J988" s="5"/>
       <c r="K988" s="1"/>
       <c r="L988" s="1"/>
       <c r="M988" s="1"/>
     </row>
     <row r="989" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A989" s="1" t="s">
-        <v>276</v>
+        <v>2201</v>
       </c>
       <c r="B989" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C989" s="1" t="s">
-        <v>1386</v>
+        <v>2084</v>
       </c>
       <c r="D989" s="1" t="s">
-        <v>1386</v>
+        <v>2084</v>
       </c>
       <c r="E989" s="1">
-        <v>8899003</v>
+        <v>6102111</v>
       </c>
       <c r="F989" s="4">
-        <v>45093.625</v>
-      </c>
-      <c r="G989" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>44286.770833333336</v>
+      </c>
+      <c r="G989" s="1"/>
       <c r="H989" s="1"/>
-      <c r="I989" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J989" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="I989" s="1"/>
+      <c r="J989" s="1"/>
       <c r="K989" s="1"/>
       <c r="L989" s="1"/>
       <c r="M989" s="1"/>
     </row>
     <row r="990" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A990" s="1" t="s">
-        <v>276</v>
+        <v>12</v>
       </c>
       <c r="B990" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C990" s="1" t="s">
-        <v>1391</v>
+        <v>2132</v>
       </c>
       <c r="D990" s="1" t="s">
-        <v>1391</v>
+        <v>2132</v>
       </c>
       <c r="E990" s="1">
-        <v>8899004</v>
-      </c>
-      <c r="F990" s="4">
-        <v>45093.5625</v>
-      </c>
-      <c r="G990" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>8927007</v>
+      </c>
+      <c r="F990" s="1"/>
+      <c r="G990" s="1"/>
       <c r="H990" s="1"/>
-      <c r="I990" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J990" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="I990" s="1"/>
+      <c r="J990" s="1"/>
       <c r="K990" s="1"/>
       <c r="L990" s="1"/>
       <c r="M990" s="1"/>
     </row>
     <row r="991" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A991" s="1" t="s">
-        <v>2203</v>
+        <v>2201</v>
       </c>
       <c r="B991" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C991" s="1" t="s">
-        <v>1423</v>
+        <v>2187</v>
       </c>
       <c r="D991" s="1" t="s">
-        <v>1423</v>
+        <v>2187</v>
       </c>
       <c r="E991" s="1">
-        <v>8808037</v>
+        <v>37001001</v>
       </c>
       <c r="F991" s="4">
-        <v>45093.666666666664</v>
-      </c>
-      <c r="G991" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>44923.458333333336</v>
+      </c>
+      <c r="G991" s="1"/>
       <c r="H991" s="1"/>
-      <c r="I991" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J991" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="I991" s="1"/>
+      <c r="J991" s="1"/>
       <c r="K991" s="1"/>
       <c r="L991" s="1"/>
       <c r="M991" s="1"/>
@@ -37271,23 +37252,21 @@
     </row>
     <row r="994" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A994" s="1" t="s">
-        <v>2203</v>
+        <v>2202</v>
       </c>
       <c r="B994" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C994" s="1" t="s">
-        <v>1429</v>
+        <v>75</v>
       </c>
       <c r="D994" s="1" t="s">
-        <v>1429</v>
+        <v>76</v>
       </c>
       <c r="E994" s="1">
-        <v>8808013</v>
-      </c>
-      <c r="F994" s="4">
-        <v>45093.625</v>
-      </c>
+        <v>4100999</v>
+      </c>
+      <c r="F994" s="1"/>
       <c r="G994" s="1" t="s">
         <v>39</v>
       </c>
@@ -37296,7 +37275,7 @@
         <v>23</v>
       </c>
       <c r="J994" s="1" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="K994" s="1"/>
       <c r="L994" s="1"/>
@@ -37304,33 +37283,27 @@
     </row>
     <row r="995" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A995" s="1" t="s">
-        <v>2203</v>
+        <v>2202</v>
       </c>
       <c r="B995" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C995" s="1" t="s">
-        <v>1484</v>
+        <v>109</v>
       </c>
       <c r="D995" s="1" t="s">
-        <v>1484</v>
+        <v>108</v>
       </c>
       <c r="E995" s="1">
-        <v>8808038</v>
+        <v>41001042</v>
       </c>
       <c r="F995" s="4">
-        <v>45093.416666666664</v>
-      </c>
-      <c r="G995" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>44292.5</v>
+      </c>
+      <c r="G995" s="1"/>
       <c r="H995" s="1"/>
-      <c r="I995" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J995" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="I995" s="1"/>
+      <c r="J995" s="1"/>
       <c r="K995" s="1"/>
       <c r="L995" s="1"/>
       <c r="M995" s="1"/>
@@ -37696,15 +37669,17 @@
         <v>37</v>
       </c>
       <c r="C1007" s="1" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="D1007" s="1" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="E1007" s="1">
-        <v>4100999</v>
-      </c>
-      <c r="F1007" s="1"/>
+        <v>41001041</v>
+      </c>
+      <c r="F1007" s="4">
+        <v>44386.6875</v>
+      </c>
       <c r="G1007" s="1" t="s">
         <v>39</v>
       </c>
@@ -37727,16 +37702,16 @@
         <v>37</v>
       </c>
       <c r="C1008" s="1" t="s">
-        <v>107</v>
+        <v>225</v>
       </c>
       <c r="D1008" s="1" t="s">
-        <v>106</v>
+        <v>224</v>
       </c>
       <c r="E1008" s="1">
-        <v>41001041</v>
+        <v>41001046</v>
       </c>
       <c r="F1008" s="4">
-        <v>44386.6875</v>
+        <v>44386.645833333336</v>
       </c>
       <c r="G1008" s="1" t="s">
         <v>39</v>
@@ -37754,22 +37729,22 @@
     </row>
     <row r="1009" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1009" s="1" t="s">
-        <v>2202</v>
+        <v>276</v>
       </c>
       <c r="B1009" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1009" s="1" t="s">
-        <v>225</v>
+        <v>310</v>
       </c>
       <c r="D1009" s="1" t="s">
-        <v>224</v>
+        <v>311</v>
       </c>
       <c r="E1009" s="1">
-        <v>41001046</v>
+        <v>8802058</v>
       </c>
       <c r="F1009" s="4">
-        <v>44386.645833333336</v>
+        <v>44894.649305555555</v>
       </c>
       <c r="G1009" s="1" t="s">
         <v>39</v>
@@ -37799,10 +37774,10 @@
         <v>311</v>
       </c>
       <c r="E1010" s="1">
-        <v>8802058</v>
+        <v>43001051</v>
       </c>
       <c r="F1010" s="4">
-        <v>44894.649305555555</v>
+        <v>44386.354166666664</v>
       </c>
       <c r="G1010" s="1" t="s">
         <v>39</v>
@@ -38277,7 +38252,7 @@
       </c>
       <c r="H1026" s="1"/>
       <c r="I1026" s="1" t="s">
-        <v>475</v>
+        <v>23</v>
       </c>
       <c r="J1026" s="1" t="s">
         <v>24</v>
@@ -39450,20 +39425,18 @@
         <v>37</v>
       </c>
       <c r="C1065" s="1" t="s">
-        <v>1285</v>
+        <v>969</v>
       </c>
       <c r="D1065" s="1" t="s">
-        <v>1285</v>
+        <v>970</v>
       </c>
       <c r="E1065" s="1">
-        <v>8348010</v>
+        <v>8800004</v>
       </c>
       <c r="F1065" s="4">
-        <v>45012.520833333336</v>
-      </c>
-      <c r="G1065" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>44771.354166666664</v>
+      </c>
+      <c r="G1065" s="1"/>
       <c r="H1065" s="1"/>
       <c r="I1065" s="1"/>
       <c r="J1065" s="1"/>
@@ -39479,20 +39452,18 @@
         <v>37</v>
       </c>
       <c r="C1066" s="1" t="s">
-        <v>1286</v>
+        <v>993</v>
       </c>
       <c r="D1066" s="1" t="s">
-        <v>1285</v>
+        <v>994</v>
       </c>
       <c r="E1066" s="1">
-        <v>45013008</v>
+        <v>8800005</v>
       </c>
       <c r="F1066" s="4">
-        <v>44368.53125</v>
-      </c>
-      <c r="G1066" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>44771.625</v>
+      </c>
+      <c r="G1066" s="1"/>
       <c r="H1066" s="1"/>
       <c r="I1066" s="1"/>
       <c r="J1066" s="1"/>
@@ -41722,64 +41693,54 @@
     </row>
     <row r="1139" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1139" s="1" t="s">
-        <v>276</v>
+        <v>12</v>
       </c>
       <c r="B1139" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1139" s="1" t="s">
-        <v>310</v>
+        <v>1016</v>
       </c>
       <c r="D1139" s="1" t="s">
-        <v>311</v>
+        <v>1017</v>
       </c>
       <c r="E1139" s="1">
-        <v>43001051</v>
+        <v>8913002</v>
       </c>
       <c r="F1139" s="4">
-        <v>44386.354166666664</v>
-      </c>
-      <c r="G1139" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>44396.625</v>
+      </c>
+      <c r="G1139" s="1"/>
       <c r="H1139" s="1"/>
-      <c r="I1139" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1139" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="I1139" s="1"/>
+      <c r="J1139" s="1"/>
       <c r="K1139" s="1"/>
       <c r="L1139" s="1"/>
       <c r="M1139" s="1"/>
     </row>
     <row r="1140" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1140" s="1" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B1140" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1140" s="1" t="s">
-        <v>1197</v>
+        <v>1020</v>
       </c>
       <c r="D1140" s="1" t="s">
-        <v>1198</v>
+        <v>1021</v>
       </c>
       <c r="E1140" s="1">
-        <v>4100901</v>
-      </c>
-      <c r="F1140" s="1"/>
-      <c r="G1140" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>8913001</v>
+      </c>
+      <c r="F1140" s="4">
+        <v>44396.5</v>
+      </c>
+      <c r="G1140" s="1"/>
       <c r="H1140" s="1"/>
-      <c r="I1140" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1140" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="I1140" s="1"/>
+      <c r="J1140" s="1"/>
       <c r="K1140" s="1"/>
       <c r="L1140" s="1"/>
       <c r="M1140" s="1"/>
@@ -42085,26 +42046,24 @@
     </row>
     <row r="1150" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1150" s="1" t="s">
-        <v>276</v>
+        <v>12</v>
       </c>
       <c r="B1150" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1150" s="1" t="s">
-        <v>1376</v>
+        <v>1018</v>
       </c>
       <c r="D1150" s="1" t="s">
-        <v>1376</v>
+        <v>1019</v>
       </c>
       <c r="E1150" s="1">
-        <v>8805032</v>
+        <v>8913003</v>
       </c>
       <c r="F1150" s="4">
-        <v>45093.541666666664</v>
-      </c>
-      <c r="G1150" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>44396.666666666664</v>
+      </c>
+      <c r="G1150" s="1"/>
       <c r="H1150" s="1"/>
       <c r="I1150" s="1"/>
       <c r="J1150" s="1"/>
@@ -42351,118 +42310,104 @@
     </row>
     <row r="1158" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1158" s="1" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B1158" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1158" s="1" t="s">
-        <v>1210</v>
+        <v>1124</v>
       </c>
       <c r="D1158" s="1" t="s">
-        <v>1209</v>
+        <v>1123</v>
       </c>
       <c r="E1158" s="1">
-        <v>41082008</v>
+        <v>41002001</v>
       </c>
       <c r="F1158" s="4">
-        <v>44386.645833333336</v>
-      </c>
-      <c r="G1158" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>44386.684027777781</v>
+      </c>
+      <c r="G1158" s="1"/>
       <c r="H1158" s="1"/>
-      <c r="I1158" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1158" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="I1158" s="1"/>
+      <c r="J1158" s="1"/>
       <c r="K1158" s="1"/>
       <c r="L1158" s="1"/>
       <c r="M1158" s="1"/>
     </row>
     <row r="1159" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1159" s="1" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B1159" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1159" s="1" t="s">
-        <v>1208</v>
+        <v>1130</v>
       </c>
       <c r="D1159" s="1" t="s">
-        <v>1207</v>
+        <v>1129</v>
       </c>
       <c r="E1159" s="1">
-        <v>41082007</v>
+        <v>41002009</v>
       </c>
       <c r="F1159" s="4">
-        <v>44386.677083333336</v>
-      </c>
-      <c r="G1159" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>44386.458333333336</v>
+      </c>
+      <c r="G1159" s="1"/>
       <c r="H1159" s="1"/>
-      <c r="I1159" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1159" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="I1159" s="1"/>
+      <c r="J1159" s="1"/>
       <c r="K1159" s="1"/>
       <c r="L1159" s="1"/>
       <c r="M1159" s="1"/>
     </row>
     <row r="1160" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1160" s="1" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B1160" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1160" s="1" t="s">
-        <v>1214</v>
+        <v>1148</v>
       </c>
       <c r="D1160" s="1" t="s">
-        <v>1213</v>
+        <v>1147</v>
       </c>
       <c r="E1160" s="1">
-        <v>41082010</v>
+        <v>41002002</v>
       </c>
       <c r="F1160" s="4">
-        <v>44386.677083333336</v>
-      </c>
-      <c r="G1160" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>44386.583333333336</v>
+      </c>
+      <c r="G1160" s="1"/>
       <c r="H1160" s="1"/>
-      <c r="I1160" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1160" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="I1160" s="1"/>
+      <c r="J1160" s="1"/>
       <c r="K1160" s="1"/>
       <c r="L1160" s="1"/>
       <c r="M1160" s="1"/>
     </row>
     <row r="1161" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1161" s="1"/>
+      <c r="A1161" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B1161" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1161" s="1" t="s">
-        <v>1390</v>
+        <v>1150</v>
       </c>
       <c r="D1161" s="1" t="s">
-        <v>1390</v>
+        <v>1149</v>
       </c>
       <c r="E1161" s="1">
-        <v>8899010</v>
-      </c>
-      <c r="F1161" s="1"/>
+        <v>41002003</v>
+      </c>
+      <c r="F1161" s="4">
+        <v>44385.5625</v>
+      </c>
       <c r="G1161" s="1"/>
       <c r="H1161" s="1"/>
       <c r="I1161" s="1"/>
@@ -42476,22 +42421,22 @@
         <v>51</v>
       </c>
       <c r="B1162" s="1" t="s">
-        <v>37</v>
+        <v>521</v>
       </c>
       <c r="C1162" s="1" t="s">
-        <v>1227</v>
+        <v>1196</v>
       </c>
       <c r="D1162" s="1" t="s">
-        <v>1226</v>
+        <v>1195</v>
       </c>
       <c r="E1162" s="1">
-        <v>41082009</v>
+        <v>41082006</v>
       </c>
       <c r="F1162" s="4">
-        <v>44386.604166666664</v>
+        <v>44385.635416666664</v>
       </c>
       <c r="G1162" s="1" t="s">
-        <v>39</v>
+        <v>202</v>
       </c>
       <c r="H1162" s="1"/>
       <c r="I1162" s="1" t="s">
@@ -42512,17 +42457,15 @@
         <v>37</v>
       </c>
       <c r="C1163" s="1" t="s">
-        <v>1229</v>
+        <v>1197</v>
       </c>
       <c r="D1163" s="1" t="s">
-        <v>1228</v>
+        <v>1198</v>
       </c>
       <c r="E1163" s="1">
-        <v>41082011</v>
-      </c>
-      <c r="F1163" s="4">
-        <v>44385.385416666664</v>
-      </c>
+        <v>4100901</v>
+      </c>
+      <c r="F1163" s="1"/>
       <c r="G1163" s="1" t="s">
         <v>39</v>
       </c>
@@ -43355,22 +43298,22 @@
     </row>
     <row r="1192" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1192" s="1" t="s">
-        <v>276</v>
+        <v>51</v>
       </c>
       <c r="B1192" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1192" s="1" t="s">
-        <v>1387</v>
+        <v>1210</v>
       </c>
       <c r="D1192" s="1" t="s">
-        <v>1386</v>
+        <v>1209</v>
       </c>
       <c r="E1192" s="1">
-        <v>43037002</v>
+        <v>41082008</v>
       </c>
       <c r="F1192" s="4">
-        <v>44386.635416666664</v>
+        <v>44386.645833333336</v>
       </c>
       <c r="G1192" s="1" t="s">
         <v>39</v>
@@ -43388,22 +43331,22 @@
     </row>
     <row r="1193" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1193" s="1" t="s">
-        <v>276</v>
+        <v>51</v>
       </c>
       <c r="B1193" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1193" s="1" t="s">
-        <v>1388</v>
+        <v>1208</v>
       </c>
       <c r="D1193" s="1" t="s">
-        <v>1389</v>
+        <v>1207</v>
       </c>
       <c r="E1193" s="1">
-        <v>43037001</v>
+        <v>41082007</v>
       </c>
       <c r="F1193" s="4">
-        <v>44386.552083333336</v>
+        <v>44386.677083333336</v>
       </c>
       <c r="G1193" s="1" t="s">
         <v>39</v>
@@ -43509,46 +43452,56 @@
       <c r="M1196" s="1"/>
     </row>
     <row r="1197" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1197" s="1"/>
+      <c r="A1197" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="B1197" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1197" s="1" t="s">
-        <v>1428</v>
+        <v>1214</v>
       </c>
       <c r="D1197" s="1" t="s">
-        <v>1428</v>
+        <v>1213</v>
       </c>
       <c r="E1197" s="1">
-        <v>8808077</v>
-      </c>
-      <c r="F1197" s="1"/>
-      <c r="G1197" s="1"/>
+        <v>41082010</v>
+      </c>
+      <c r="F1197" s="4">
+        <v>44386.677083333336</v>
+      </c>
+      <c r="G1197" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H1197" s="1"/>
-      <c r="I1197" s="1"/>
-      <c r="J1197" s="1"/>
+      <c r="I1197" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1197" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K1197" s="1"/>
       <c r="L1197" s="1"/>
       <c r="M1197" s="1"/>
     </row>
     <row r="1198" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1198" s="1" t="s">
-        <v>276</v>
+        <v>51</v>
       </c>
       <c r="B1198" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1198" s="1" t="s">
-        <v>1392</v>
+        <v>1227</v>
       </c>
       <c r="D1198" s="1" t="s">
-        <v>1391</v>
+        <v>1226</v>
       </c>
       <c r="E1198" s="1">
-        <v>43037003</v>
+        <v>41082009</v>
       </c>
       <c r="F1198" s="4">
-        <v>44386.583333333336</v>
+        <v>44386.604166666664</v>
       </c>
       <c r="G1198" s="1" t="s">
         <v>39</v>
@@ -43566,22 +43519,22 @@
     </row>
     <row r="1199" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1199" s="1" t="s">
-        <v>2203</v>
+        <v>51</v>
       </c>
       <c r="B1199" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1199" s="1" t="s">
-        <v>1424</v>
+        <v>1229</v>
       </c>
       <c r="D1199" s="1" t="s">
-        <v>1423</v>
+        <v>1228</v>
       </c>
       <c r="E1199" s="1">
-        <v>43006037</v>
+        <v>41082011</v>
       </c>
       <c r="F1199" s="4">
-        <v>44386.65625</v>
+        <v>44385.385416666664</v>
       </c>
       <c r="G1199" s="1" t="s">
         <v>39</v>
@@ -44485,16 +44438,10 @@
       <c r="F1231" s="4">
         <v>45092.5</v>
       </c>
-      <c r="G1231" s="1" t="s">
-        <v>122</v>
-      </c>
+      <c r="G1231" s="1"/>
       <c r="H1231" s="1"/>
-      <c r="I1231" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1231" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="I1231" s="1"/>
+      <c r="J1231" s="1"/>
       <c r="K1231" s="1"/>
       <c r="L1231" s="1"/>
       <c r="M1231" s="1"/>
@@ -44518,16 +44465,10 @@
       <c r="F1232" s="4">
         <v>44385.416666666664</v>
       </c>
-      <c r="G1232" s="1" t="s">
-        <v>122</v>
-      </c>
+      <c r="G1232" s="1"/>
       <c r="H1232" s="1"/>
-      <c r="I1232" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1232" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="I1232" s="1"/>
+      <c r="J1232" s="1"/>
       <c r="K1232" s="1"/>
       <c r="L1232" s="1"/>
       <c r="M1232" s="1"/>
@@ -45108,55 +45049,49 @@
     </row>
     <row r="1251" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1251" s="1" t="s">
-        <v>2203</v>
+        <v>12</v>
       </c>
       <c r="B1251" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1251" s="1" t="s">
-        <v>1430</v>
+        <v>1286</v>
       </c>
       <c r="D1251" s="1" t="s">
-        <v>1429</v>
+        <v>1285</v>
       </c>
       <c r="E1251" s="1">
-        <v>43006013</v>
+        <v>45013008</v>
       </c>
       <c r="F1251" s="4">
-        <v>44386.645833333336</v>
-      </c>
-      <c r="G1251" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>44368.53125</v>
+      </c>
+      <c r="G1251" s="1"/>
       <c r="H1251" s="1"/>
-      <c r="I1251" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1251" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="I1251" s="1"/>
+      <c r="J1251" s="1"/>
       <c r="K1251" s="1"/>
       <c r="L1251" s="1"/>
       <c r="M1251" s="1"/>
     </row>
     <row r="1252" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1252" s="1" t="s">
-        <v>2203</v>
+        <v>276</v>
       </c>
       <c r="B1252" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1252" s="1" t="s">
-        <v>1485</v>
+        <v>1387</v>
       </c>
       <c r="D1252" s="1" t="s">
-        <v>1484</v>
+        <v>1386</v>
       </c>
       <c r="E1252" s="1">
-        <v>43006038</v>
+        <v>43037002</v>
       </c>
       <c r="F1252" s="4">
-        <v>44386.4375</v>
+        <v>44386.635416666664</v>
       </c>
       <c r="G1252" s="1" t="s">
         <v>39</v>
@@ -46758,29 +46693,33 @@
     </row>
     <row r="1305" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1305" s="1" t="s">
-        <v>12</v>
+        <v>276</v>
       </c>
       <c r="B1305" s="1" t="s">
-        <v>642</v>
+        <v>37</v>
       </c>
       <c r="C1305" s="1" t="s">
-        <v>1540</v>
+        <v>1388</v>
       </c>
       <c r="D1305" s="1" t="s">
-        <v>1540</v>
+        <v>1389</v>
       </c>
       <c r="E1305" s="1">
-        <v>8849007</v>
+        <v>43037001</v>
       </c>
       <c r="F1305" s="4">
-        <v>45093.6875</v>
+        <v>44386.552083333336</v>
       </c>
       <c r="G1305" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H1305" s="1"/>
-      <c r="I1305" s="1"/>
-      <c r="J1305" s="1"/>
+      <c r="I1305" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1305" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K1305" s="1"/>
       <c r="L1305" s="1"/>
       <c r="M1305" s="1"/>
@@ -47930,29 +47869,33 @@
     </row>
     <row r="1347" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1347" s="1" t="s">
-        <v>16</v>
+        <v>276</v>
       </c>
       <c r="B1347" s="1" t="s">
-        <v>642</v>
+        <v>37</v>
       </c>
       <c r="C1347" s="1" t="s">
-        <v>1585</v>
+        <v>1392</v>
       </c>
       <c r="D1347" s="1" t="s">
-        <v>1585</v>
+        <v>1391</v>
       </c>
       <c r="E1347" s="1">
-        <v>8001061</v>
+        <v>43037003</v>
       </c>
       <c r="F1347" s="4">
-        <v>45063.5</v>
+        <v>44386.583333333336</v>
       </c>
       <c r="G1347" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H1347" s="1"/>
-      <c r="I1347" s="1"/>
-      <c r="J1347" s="1"/>
+      <c r="I1347" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1347" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K1347" s="1"/>
       <c r="L1347" s="1"/>
       <c r="M1347" s="1"/>
@@ -47994,22 +47937,22 @@
     </row>
     <row r="1349" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1349" s="1" t="s">
-        <v>16</v>
+        <v>2202</v>
       </c>
       <c r="B1349" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C1349" s="1" t="s">
-        <v>1587</v>
+        <v>255</v>
       </c>
       <c r="D1349" s="1" t="s">
-        <v>1587</v>
+        <v>254</v>
       </c>
       <c r="E1349" s="1">
-        <v>8001032</v>
+        <v>41001033</v>
       </c>
       <c r="F1349" s="4">
-        <v>45094.645833333336</v>
+        <v>44386.6875</v>
       </c>
       <c r="G1349" s="1" t="s">
         <v>248</v>
@@ -48027,22 +47970,22 @@
     </row>
     <row r="1350" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1350" s="1" t="s">
-        <v>16</v>
+        <v>2202</v>
       </c>
       <c r="B1350" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C1350" s="1" t="s">
-        <v>1588</v>
+        <v>257</v>
       </c>
       <c r="D1350" s="1" t="s">
-        <v>1588</v>
+        <v>256</v>
       </c>
       <c r="E1350" s="1">
-        <v>8001031</v>
+        <v>41001037</v>
       </c>
       <c r="F1350" s="4">
-        <v>45093.583333333336</v>
+        <v>44385.666666666664</v>
       </c>
       <c r="G1350" s="1" t="s">
         <v>248</v>
@@ -48060,22 +48003,22 @@
     </row>
     <row r="1351" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1351" s="1" t="s">
-        <v>16</v>
+        <v>2202</v>
       </c>
       <c r="B1351" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C1351" s="1" t="s">
-        <v>1589</v>
+        <v>264</v>
       </c>
       <c r="D1351" s="1" t="s">
-        <v>1589</v>
+        <v>263</v>
       </c>
       <c r="E1351" s="1">
-        <v>8001030</v>
+        <v>41001036</v>
       </c>
       <c r="F1351" s="4">
-        <v>45094.666666666664</v>
+        <v>44385.6875</v>
       </c>
       <c r="G1351" s="1" t="s">
         <v>248</v>
@@ -48668,22 +48611,22 @@
     </row>
     <row r="1369" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1369" s="1" t="s">
-        <v>16</v>
+        <v>276</v>
       </c>
       <c r="B1369" s="1" t="s">
-        <v>505</v>
+        <v>248</v>
       </c>
       <c r="C1369" s="1" t="s">
-        <v>1608</v>
+        <v>320</v>
       </c>
       <c r="D1369" s="1" t="s">
-        <v>1608</v>
+        <v>319</v>
       </c>
       <c r="E1369" s="1">
-        <v>8001021</v>
+        <v>43001049</v>
       </c>
       <c r="F1369" s="4">
-        <v>45093.645833333336</v>
+        <v>44386.625</v>
       </c>
       <c r="G1369" s="1" t="s">
         <v>248</v>
@@ -49565,22 +49508,22 @@
     </row>
     <row r="1396" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1396" s="1" t="s">
-        <v>16</v>
+        <v>276</v>
       </c>
       <c r="B1396" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C1396" s="1" t="s">
-        <v>1637</v>
+        <v>322</v>
       </c>
       <c r="D1396" s="1" t="s">
-        <v>1637</v>
+        <v>321</v>
       </c>
       <c r="E1396" s="1">
-        <v>8001088</v>
+        <v>43001046</v>
       </c>
       <c r="F1396" s="4">
-        <v>45092.458333333336</v>
+        <v>44386.708333333336</v>
       </c>
       <c r="G1396" s="1" t="s">
         <v>248</v>
@@ -49598,22 +49541,22 @@
     </row>
     <row r="1397" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1397" s="1" t="s">
-        <v>16</v>
+        <v>2203</v>
       </c>
       <c r="B1397" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C1397" s="1" t="s">
-        <v>1638</v>
+        <v>436</v>
       </c>
       <c r="D1397" s="1" t="s">
-        <v>1638</v>
+        <v>435</v>
       </c>
       <c r="E1397" s="1">
-        <v>8001084</v>
+        <v>43002007</v>
       </c>
       <c r="F1397" s="4">
-        <v>45084.666666666664</v>
+        <v>44385.583333333336</v>
       </c>
       <c r="G1397" s="1" t="s">
         <v>248</v>
@@ -61063,29 +61006,33 @@
     </row>
     <row r="1780" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1780" s="1" t="s">
-        <v>2201</v>
+        <v>2203</v>
       </c>
       <c r="B1780" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1780" s="1" t="s">
-        <v>2084</v>
+        <v>1424</v>
       </c>
       <c r="D1780" s="1" t="s">
-        <v>2084</v>
+        <v>1423</v>
       </c>
       <c r="E1780" s="1">
-        <v>6102111</v>
+        <v>43006037</v>
       </c>
       <c r="F1780" s="4">
-        <v>44286.770833333336</v>
+        <v>44386.65625</v>
       </c>
       <c r="G1780" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H1780" s="1"/>
-      <c r="I1780" s="1"/>
-      <c r="J1780" s="1"/>
+      <c r="I1780" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1780" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K1780" s="1"/>
       <c r="L1780" s="1"/>
       <c r="M1780" s="1"/>
@@ -61488,27 +61435,33 @@
     </row>
     <row r="1795" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1795" s="1" t="s">
-        <v>12</v>
+        <v>2203</v>
       </c>
       <c r="B1795" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1795" s="1" t="s">
-        <v>2102</v>
+        <v>1430</v>
       </c>
       <c r="D1795" s="1" t="s">
-        <v>2103</v>
+        <v>1429</v>
       </c>
       <c r="E1795" s="1">
-        <v>2101041</v>
-      </c>
-      <c r="F1795" s="1"/>
+        <v>43006013</v>
+      </c>
+      <c r="F1795" s="4">
+        <v>44386.645833333336</v>
+      </c>
       <c r="G1795" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H1795" s="1"/>
-      <c r="I1795" s="1"/>
-      <c r="J1795" s="1"/>
+      <c r="I1795" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1795" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K1795" s="1"/>
       <c r="L1795" s="1"/>
       <c r="M1795" s="1"/>
@@ -62108,27 +62061,33 @@
     </row>
     <row r="1817" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1817" s="1" t="s">
-        <v>12</v>
+        <v>2203</v>
       </c>
       <c r="B1817" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1817" s="1" t="s">
-        <v>2132</v>
+        <v>1485</v>
       </c>
       <c r="D1817" s="1" t="s">
-        <v>2132</v>
+        <v>1484</v>
       </c>
       <c r="E1817" s="1">
-        <v>8927007</v>
-      </c>
-      <c r="F1817" s="1"/>
+        <v>43006038</v>
+      </c>
+      <c r="F1817" s="4">
+        <v>44386.4375</v>
+      </c>
       <c r="G1817" s="1" t="s">
         <v>39</v>
       </c>
       <c r="H1817" s="1"/>
-      <c r="I1817" s="1"/>
-      <c r="J1817" s="1"/>
+      <c r="I1817" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1817" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="K1817" s="1"/>
       <c r="L1817" s="1"/>
       <c r="M1817" s="1"/>
@@ -63289,26 +63248,22 @@
     </row>
     <row r="1858" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1858" s="1" t="s">
-        <v>2201</v>
+        <v>12</v>
       </c>
       <c r="B1858" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C1858" s="1" t="s">
-        <v>2187</v>
+        <v>2102</v>
       </c>
       <c r="D1858" s="1" t="s">
-        <v>2187</v>
+        <v>2103</v>
       </c>
       <c r="E1858" s="1">
-        <v>37001001</v>
-      </c>
-      <c r="F1858" s="4">
-        <v>44923.458333333336</v>
-      </c>
-      <c r="G1858" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>2101041</v>
+      </c>
+      <c r="F1858" s="1"/>
+      <c r="G1858" s="1"/>
       <c r="H1858" s="1"/>
       <c r="I1858" s="1"/>
       <c r="J1858" s="1"/>
@@ -63519,9 +63474,79 @@
       <c r="L1865" s="1"/>
       <c r="M1865" s="1"/>
     </row>
+    <row r="1866" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1866" t="s">
+        <v>2210</v>
+      </c>
+      <c r="B1866" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1866" s="7" t="s">
+        <v>2211</v>
+      </c>
+      <c r="D1866" s="7" t="s">
+        <v>2211</v>
+      </c>
+      <c r="E1866" s="8">
+        <v>8718004</v>
+      </c>
+      <c r="G1866" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1866" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1866" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1867" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1867" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1867" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1867" s="8" t="s">
+        <v>2212</v>
+      </c>
+      <c r="D1867" s="8" t="s">
+        <v>2212</v>
+      </c>
+      <c r="E1867" s="8">
+        <v>8811028</v>
+      </c>
+    </row>
+    <row r="1868" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1868" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1868" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1868" s="8" t="s">
+        <v>2213</v>
+      </c>
+      <c r="D1868" s="8" t="s">
+        <v>2213</v>
+      </c>
+      <c r="E1868" s="8">
+        <v>8849050</v>
+      </c>
+      <c r="G1868" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1868" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1868" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M1865"/>
+  <autoFilter ref="A1:M1868"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>